<commit_message>
updated treatment of Rhynie mites based on Klimov et al. 2025
</commit_message>
<xml_diff>
--- a/RhynieGuildStructure.xlsx
+++ b/RhynieGuildStructure.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tannerfrank/Dropbox/Work/Devonian terr ecosystems/EcolNetworks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tannerfrank/Dropbox/Work/Devonian terr ecosystems/EcolNetworks/RhynieWebRepo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{134FA0A4-64F5-EB46-8521-05B18411DC3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0970A460-2D43-704D-9A28-AE8437D0F48E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="680" windowWidth="14400" windowHeight="16380" xr2:uid="{917E407B-513B-1147-91E2-A7CD7550F694}"/>
   </bookViews>
   <sheets>
-    <sheet name="Guild definitions" sheetId="3" r:id="rId1"/>
-    <sheet name="Guild compositions" sheetId="2" r:id="rId2"/>
+    <sheet name="Guilds" sheetId="3" r:id="rId1"/>
+    <sheet name="Guild composition" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="179">
   <si>
     <t>terrestrial detritus</t>
   </si>
@@ -210,15 +210,6 @@
     <t>Protacarus crani</t>
   </si>
   <si>
-    <t>Paraprotacarus hirsti</t>
-  </si>
-  <si>
-    <t>Palaeotydeus devonicus</t>
-  </si>
-  <si>
-    <t>Protospeleorchestes pseudoprotacarus</t>
-  </si>
-  <si>
     <t>Pseudoprotacarus scoticus</t>
   </si>
   <si>
@@ -525,9 +516,6 @@
     <t>terrestrial microbivores</t>
   </si>
   <si>
-    <t>herbivore mites</t>
-  </si>
-  <si>
     <t>24?,11,10,9?,8</t>
   </si>
   <si>
@@ -549,12 +537,6 @@
     <t>28,27,26,25,24?,20?,19?,18?,17?,13</t>
   </si>
   <si>
-    <t>20,19?,7?,6,5,4,3,2,1?</t>
-  </si>
-  <si>
-    <t>7?,6,5?,4,1?, 21?</t>
-  </si>
-  <si>
     <t>0?</t>
   </si>
   <si>
@@ -583,6 +565,15 @@
   </si>
   <si>
     <t>resource_guilds</t>
+  </si>
+  <si>
+    <t>mites</t>
+  </si>
+  <si>
+    <t>24, 20,7?,6,5,4,3,2?,1?</t>
+  </si>
+  <si>
+    <t>21?, 7?,6,5?,4,1?</t>
   </si>
 </sst>
 </file>
@@ -971,36 +962,37 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="37" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.83203125" customWidth="1"/>
     <col min="5" max="5" width="42.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>181</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -1011,13 +1003,13 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F2" s="2">
         <v>1</v>
@@ -1034,7 +1026,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D3" s="2">
         <v>8</v>
@@ -1076,7 +1068,7 @@
         <v>23</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D5" s="2">
         <v>17</v>
@@ -1099,13 +1091,13 @@
         <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D6" s="2">
         <v>9</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F6" s="2">
         <v>1</v>
@@ -1122,13 +1114,13 @@
         <v>18</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D7" s="2">
         <v>7</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F7" s="2">
         <v>1</v>
@@ -1145,19 +1137,19 @@
         <v>19</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D8" s="2">
         <v>3</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="F8" s="2">
         <v>1</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -1165,16 +1157,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D9" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F9" s="2">
         <v>1</v>
@@ -1191,13 +1183,13 @@
         <v>3</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D10" s="2">
         <v>2</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="F10" s="2">
         <v>1</v>
@@ -1211,16 +1203,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>162</v>
+        <v>176</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D11" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="F11" s="2">
         <v>1</v>
@@ -1237,13 +1229,13 @@
         <v>5</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D12" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="F12" s="2">
         <v>1</v>
@@ -1260,13 +1252,13 @@
         <v>6</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D13" s="2">
         <v>5</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F13" s="2">
         <v>1</v>
@@ -1283,13 +1275,13 @@
         <v>7</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D14" s="2">
         <v>1</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F14" s="2">
         <v>0</v>
@@ -1310,7 +1302,7 @@
         <v>3</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F15" s="2">
         <v>0</v>
@@ -1327,7 +1319,7 @@
         <v>16</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D16" s="2">
         <v>5</v>
@@ -1348,7 +1340,7 @@
         <v>17</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D17" s="2">
         <v>1</v>
@@ -1369,7 +1361,7 @@
         <v>8</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D18" s="2">
         <v>4</v>
@@ -1387,10 +1379,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D19" s="2">
         <v>5</v>
@@ -1411,7 +1403,7 @@
         <v>9</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D20" s="2">
         <v>1</v>
@@ -1429,10 +1421,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D21" s="2">
         <v>3</v>
@@ -1453,7 +1445,7 @@
         <v>22</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D22" s="2">
         <v>4</v>
@@ -1476,13 +1468,13 @@
         <v>20</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D23" s="2">
         <v>1</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F23" s="2">
         <v>0</v>
@@ -1496,16 +1488,16 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D24" s="2">
         <v>1</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="F24" s="2">
         <v>0</v>
@@ -1528,7 +1520,7 @@
         <v>1</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F25" s="2">
         <v>1</v>
@@ -1545,13 +1537,13 @@
         <v>15</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D26" s="2">
         <v>2</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F26" s="2">
         <v>0</v>
@@ -1568,13 +1560,13 @@
         <v>39</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D27" s="2">
         <v>1</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F27" s="2">
         <v>0</v>
@@ -1588,16 +1580,16 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D28" s="2">
         <v>2</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="F28" s="2">
         <v>0</v>
@@ -1614,13 +1606,13 @@
         <v>14</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D29" s="2">
         <v>1</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F29" s="2">
         <v>0</v>
@@ -1636,10 +1628,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC34C16-BDAC-5F40-B6B3-028EA14891F7}">
-  <dimension ref="A1:D127"/>
+  <dimension ref="A1:D124"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="F117" sqref="F117"/>
+    <sheetView topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1659,7 +1651,7 @@
         <v>26</v>
       </c>
       <c r="D1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1683,7 +1675,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C4">
         <v>8</v>
@@ -1726,7 +1718,7 @@
     </row>
     <row r="12" spans="1:4" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="C12" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -1742,15 +1734,15 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C14" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C15" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1766,17 +1758,17 @@
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C17" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C18" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C19" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D19" t="s">
         <v>42</v>
@@ -1784,7 +1776,7 @@
     </row>
     <row r="20" spans="3:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C20" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>42</v>
@@ -1792,7 +1784,7 @@
     </row>
     <row r="21" spans="3:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C21" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>42</v>
@@ -1800,7 +1792,7 @@
     </row>
     <row r="22" spans="3:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C22" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>42</v>
@@ -1808,7 +1800,7 @@
     </row>
     <row r="23" spans="3:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C23" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>42</v>
@@ -1816,7 +1808,7 @@
     </row>
     <row r="24" spans="3:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C24" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>42</v>
@@ -1824,42 +1816,42 @@
     </row>
     <row r="25" spans="3:4" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="C25" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C26" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C27" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C28" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C29" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C30" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C31" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C32" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D32" t="s">
         <v>42</v>
@@ -1878,47 +1870,47 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C34" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C35" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C36" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C37" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="38" spans="1:4" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="C38" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="39" spans="1:4" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="C39" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="40" spans="1:4" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="C40" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="41" spans="1:4" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="C41" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="42" spans="1:4" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="C42" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -1934,7 +1926,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C44" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D44" t="s">
         <v>42</v>
@@ -1942,12 +1934,12 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C45" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="46" spans="1:4" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="C46" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>42</v>
@@ -1955,22 +1947,22 @@
     </row>
     <row r="47" spans="1:4" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="C47" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="48" spans="1:4" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="C48" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="49" spans="1:4" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="C49" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="50" spans="1:4" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="C50" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>42</v>
@@ -1989,12 +1981,12 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C52" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C53" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D53" t="s">
         <v>42</v>
@@ -2002,7 +1994,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C54" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
@@ -2013,7 +2005,7 @@
         <v>4</v>
       </c>
       <c r="C55">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
@@ -2022,43 +2014,46 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C57" t="s">
-        <v>60</v>
+      <c r="A57">
+        <v>9</v>
+      </c>
+      <c r="B57" t="s">
+        <v>3</v>
+      </c>
+      <c r="C57">
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58">
-        <v>9</v>
-      </c>
-      <c r="B58" t="s">
-        <v>3</v>
-      </c>
-      <c r="C58">
-        <v>2</v>
+      <c r="C58" t="s">
+        <v>49</v>
+      </c>
+      <c r="D58" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C59" t="s">
-        <v>49</v>
-      </c>
-      <c r="D59" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>10</v>
+      </c>
+      <c r="B60" t="s">
+        <v>176</v>
+      </c>
+      <c r="C60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C61" t="s">
+        <v>56</v>
+      </c>
+      <c r="D61" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C60" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61">
-        <v>10</v>
-      </c>
-      <c r="B61" t="s">
-        <v>162</v>
-      </c>
-      <c r="C61">
-        <v>3</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
@@ -2070,477 +2065,453 @@
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C63" t="s">
-        <v>58</v>
-      </c>
-      <c r="D63" t="s">
-        <v>42</v>
+      <c r="A63">
+        <v>11</v>
+      </c>
+      <c r="B63" t="s">
+        <v>5</v>
+      </c>
+      <c r="C63">
+        <v>3</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C64" t="s">
-        <v>59</v>
-      </c>
-      <c r="D64" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65">
-        <v>11</v>
-      </c>
-      <c r="B65" t="s">
-        <v>5</v>
-      </c>
-      <c r="C65">
-        <v>4</v>
+      <c r="C65" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C66" t="s">
-        <v>56</v>
-      </c>
-      <c r="D66" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C67" t="s">
-        <v>51</v>
+      <c r="A67">
+        <v>12</v>
+      </c>
+      <c r="B67" t="s">
+        <v>6</v>
+      </c>
+      <c r="C67">
+        <v>5</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C68" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C69" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70">
-        <v>12</v>
-      </c>
-      <c r="B70" t="s">
-        <v>6</v>
-      </c>
-      <c r="C70">
-        <v>5</v>
+      <c r="C70" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C71" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C72" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C73" t="s">
-        <v>61</v>
+      <c r="A73">
+        <v>13</v>
+      </c>
+      <c r="B73" t="s">
+        <v>7</v>
+      </c>
+      <c r="C73">
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C74" t="s">
-        <v>50</v>
+        <v>103</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C75" t="s">
-        <v>52</v>
+      <c r="A75">
+        <v>14</v>
+      </c>
+      <c r="B75" t="s">
+        <v>24</v>
+      </c>
+      <c r="C75">
+        <v>3</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76">
-        <v>13</v>
-      </c>
-      <c r="B76" t="s">
-        <v>7</v>
-      </c>
-      <c r="C76">
-        <v>1</v>
+      <c r="C76" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C77" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C78" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>15</v>
+      </c>
+      <c r="B79" t="s">
+        <v>113</v>
+      </c>
+      <c r="C79">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C80" s="1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78">
-        <v>14</v>
-      </c>
-      <c r="B78" t="s">
-        <v>24</v>
-      </c>
-      <c r="C78">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C79" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C80" t="s">
-        <v>124</v>
+      <c r="D80" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C81" s="1" t="s">
-        <v>13</v>
+        <v>114</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A82">
-        <v>15</v>
-      </c>
-      <c r="B82" t="s">
-        <v>116</v>
-      </c>
-      <c r="C82">
-        <v>5</v>
+      <c r="C82" s="1" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C83" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D83" t="s">
-        <v>42</v>
+        <v>127</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C84" s="1" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C85" s="1" t="s">
-        <v>129</v>
+      <c r="A85">
+        <v>16</v>
+      </c>
+      <c r="B85" t="s">
+        <v>17</v>
+      </c>
+      <c r="C85">
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C86" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C87" s="1" t="s">
-        <v>131</v>
+      <c r="A87">
+        <v>17</v>
+      </c>
+      <c r="B87" t="s">
+        <v>8</v>
+      </c>
+      <c r="C87">
+        <v>4</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A88">
-        <v>16</v>
-      </c>
-      <c r="B88" t="s">
-        <v>17</v>
-      </c>
-      <c r="C88">
-        <v>1</v>
+      <c r="C88" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D88" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C89" s="1" t="s">
-        <v>134</v>
+        <v>109</v>
+      </c>
+      <c r="D89" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A90">
-        <v>17</v>
-      </c>
-      <c r="B90" t="s">
-        <v>8</v>
-      </c>
-      <c r="C90">
-        <v>4</v>
+      <c r="C90" s="1" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C91" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D91" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>18</v>
+      </c>
+      <c r="B92" t="s">
         <v>111</v>
       </c>
-      <c r="D91" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C92" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D92" t="s">
-        <v>113</v>
+      <c r="C92">
+        <v>5</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C93" s="1" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C94" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D94" t="s">
-        <v>42</v>
+        <v>115</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A95">
-        <v>18</v>
-      </c>
-      <c r="B95" t="s">
-        <v>114</v>
-      </c>
-      <c r="C95">
-        <v>5</v>
+      <c r="C95" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D95" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C96" s="1" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C97" s="1" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C98" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D98" t="s">
-        <v>120</v>
+      <c r="A98">
+        <v>19</v>
+      </c>
+      <c r="B98" t="s">
+        <v>9</v>
+      </c>
+      <c r="C98">
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C99" s="1" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C100" s="1" t="s">
-        <v>135</v>
+      <c r="A100">
+        <v>20</v>
+      </c>
+      <c r="B100" t="s">
+        <v>112</v>
+      </c>
+      <c r="C100" s="1">
+        <v>3</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A101">
-        <v>19</v>
-      </c>
-      <c r="B101" t="s">
-        <v>9</v>
-      </c>
-      <c r="C101">
-        <v>1</v>
+      <c r="C101" s="1" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C102" s="1" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A103">
-        <v>20</v>
-      </c>
-      <c r="B103" t="s">
-        <v>115</v>
-      </c>
-      <c r="C103" s="1">
-        <v>3</v>
+      <c r="C103" s="1" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C104" s="1" t="s">
-        <v>126</v>
+      <c r="A104">
+        <v>21</v>
+      </c>
+      <c r="B104" t="s">
+        <v>22</v>
+      </c>
+      <c r="C104">
+        <v>4</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C105" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="C106" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="C107" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="C108" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <v>22</v>
+      </c>
+      <c r="B109" t="s">
+        <v>20</v>
+      </c>
+      <c r="C109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C110" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A111">
+        <v>23</v>
+      </c>
+      <c r="B111" t="s">
+        <v>21</v>
+      </c>
+      <c r="C111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C112" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <v>24</v>
+      </c>
+      <c r="B113" t="s">
+        <v>11</v>
+      </c>
+      <c r="C113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C114" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A107">
-        <v>21</v>
-      </c>
-      <c r="B107" t="s">
-        <v>22</v>
-      </c>
-      <c r="C107">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C108" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="C109" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D109" s="1" t="s">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>25</v>
+      </c>
+      <c r="B115" t="s">
+        <v>15</v>
+      </c>
+      <c r="C115">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C116" t="s">
+        <v>44</v>
+      </c>
+      <c r="D116" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="110" spans="1:4" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="C110" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D110" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="C111" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D111" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A112">
-        <v>22</v>
-      </c>
-      <c r="B112" t="s">
-        <v>20</v>
-      </c>
-      <c r="C112">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C113" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A114">
-        <v>23</v>
-      </c>
-      <c r="B114" t="s">
-        <v>21</v>
-      </c>
-      <c r="C114">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C115" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A116">
-        <v>24</v>
-      </c>
-      <c r="B116" t="s">
-        <v>11</v>
-      </c>
-      <c r="C116">
-        <v>1</v>
-      </c>
-    </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C117" s="1" t="s">
-        <v>136</v>
+      <c r="C117" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B118" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="C118">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C119" t="s">
-        <v>44</v>
-      </c>
-      <c r="D119" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <v>27</v>
+      </c>
+      <c r="B120" t="s">
+        <v>38</v>
+      </c>
+      <c r="C120">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C121" t="s">
+        <v>41</v>
+      </c>
+      <c r="D121" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C120" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A121">
-        <v>26</v>
-      </c>
-      <c r="B121" t="s">
-        <v>39</v>
-      </c>
-      <c r="C121">
-        <v>1</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C122" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B123" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="C123">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C124" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D124" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C125" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A126">
-        <v>28</v>
-      </c>
-      <c r="B126" t="s">
-        <v>14</v>
-      </c>
-      <c r="C126">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C127" t="s">
-        <v>43</v>
-      </c>
-      <c r="D127" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added lumped guild framwork files and ran analyses with them
</commit_message>
<xml_diff>
--- a/RhynieGuildStructure.xlsx
+++ b/RhynieGuildStructure.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tannerfrank/Dropbox/Work/Devonian terr ecosystems/EcolNetworks/RhynieWebRepo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0970A460-2D43-704D-9A28-AE8437D0F48E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{699FACF5-EDB0-1543-A5EE-7492F9D3ABD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="680" windowWidth="14400" windowHeight="16380" xr2:uid="{917E407B-513B-1147-91E2-A7CD7550F694}"/>
   </bookViews>
@@ -495,9 +495,6 @@
     <t>28,27,26,25,24,23,22,21,20,19,18,17,16,15,14,2,1</t>
   </si>
   <si>
-    <t>20,19?,18?,17?,16?,15?,14?,7?,6?,5?,4?,3?,2??</t>
-  </si>
-  <si>
     <t>22,15,14</t>
   </si>
   <si>
@@ -574,6 +571,9 @@
   </si>
   <si>
     <t>21?, 7?,6,5?,4,1?</t>
+  </si>
+  <si>
+    <t>2,20,19?,18?,17?,16?,15?,14?,7?,6?,5?,4?,3?</t>
   </si>
 </sst>
 </file>
@@ -962,7 +962,7 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -974,25 +974,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>172</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -1009,7 +1009,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F2" s="2">
         <v>1</v>
@@ -1143,13 +1143,13 @@
         <v>3</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F8" s="2">
         <v>1</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -1157,10 +1157,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D9" s="2">
         <v>1</v>
@@ -1189,7 +1189,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F10" s="2">
         <v>1</v>
@@ -1203,16 +1203,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D11" s="2">
         <v>2</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F11" s="2">
         <v>1</v>
@@ -1235,7 +1235,7 @@
         <v>3</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F12" s="2">
         <v>1</v>
@@ -1258,7 +1258,7 @@
         <v>5</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F13" s="2">
         <v>1</v>
@@ -1302,7 +1302,7 @@
         <v>3</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F15" s="2">
         <v>0</v>
@@ -1488,7 +1488,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>136</v>
@@ -1497,7 +1497,7 @@
         <v>1</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F24" s="2">
         <v>0</v>
@@ -1520,7 +1520,7 @@
         <v>1</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>152</v>
+        <v>178</v>
       </c>
       <c r="F25" s="2">
         <v>1</v>
@@ -1543,7 +1543,7 @@
         <v>2</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F26" s="2">
         <v>0</v>
@@ -1566,7 +1566,7 @@
         <v>1</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F27" s="2">
         <v>0</v>
@@ -1580,7 +1580,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>146</v>
@@ -1589,7 +1589,7 @@
         <v>2</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F28" s="2">
         <v>0</v>
@@ -1630,7 +1630,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC34C16-BDAC-5F40-B6B3-028EA14891F7}">
   <dimension ref="A1:D124"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
+    <sheetView topLeftCell="A62" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -1651,7 +1651,7 @@
         <v>26</v>
       </c>
       <c r="D1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2042,7 +2042,7 @@
         <v>10</v>
       </c>
       <c r="B60" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C60">
         <v>2</v>

</xml_diff>

<commit_message>
Added TrophSpLumper to lump spp w/ identical predators and prey
</commit_message>
<xml_diff>
--- a/RhynieGuildStructure.xlsx
+++ b/RhynieGuildStructure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tannerfrank/Dropbox/Work/Devonian terr ecosystems/EcolNetworks/RhynieWebRepo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tannerfrank/Library/CloudStorage/Dropbox/Work/Devonian terr ecosystems/EcolNetworks/RhynieWebRepo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{699FACF5-EDB0-1543-A5EE-7492F9D3ABD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A77E7818-B93E-5748-9FA5-22537E70A7B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="680" windowWidth="14400" windowHeight="16380" xr2:uid="{917E407B-513B-1147-91E2-A7CD7550F694}"/>
+    <workbookView xWindow="-33920" yWindow="6940" windowWidth="14400" windowHeight="16380" activeTab="1" xr2:uid="{917E407B-513B-1147-91E2-A7CD7550F694}"/>
   </bookViews>
   <sheets>
     <sheet name="Guilds" sheetId="3" r:id="rId1"/>
@@ -961,7 +961,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63A68499-41B5-0044-B3AC-D073A84B94F6}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
@@ -1630,8 +1630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC34C16-BDAC-5F40-B6B3-028EA14891F7}">
   <dimension ref="A1:D124"/>
   <sheetViews>
-    <sheetView topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Made EcoWeb Trophic species
</commit_message>
<xml_diff>
--- a/RhynieGuildStructure.xlsx
+++ b/RhynieGuildStructure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tannerfrank/Library/CloudStorage/Dropbox/Work/Devonian terr ecosystems/EcolNetworks/RhynieWebRepo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tannerfrank/Dropbox/Work/Devonian terr ecosystems/EcolNetworks/RhynieWebRepo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A77E7818-B93E-5748-9FA5-22537E70A7B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21498FD4-B9F6-594A-9051-BEC7B1935A4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33920" yWindow="6940" windowWidth="14400" windowHeight="16380" activeTab="1" xr2:uid="{917E407B-513B-1147-91E2-A7CD7550F694}"/>
+    <workbookView xWindow="18800" yWindow="680" windowWidth="10000" windowHeight="16460" activeTab="1" xr2:uid="{917E407B-513B-1147-91E2-A7CD7550F694}"/>
   </bookViews>
   <sheets>
     <sheet name="Guilds" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="180">
   <si>
     <t>terrestrial detritus</t>
   </si>
@@ -574,6 +574,9 @@
   </si>
   <si>
     <t>2,20,19?,18?,17?,16?,15?,14?,7?,6?,5?,4?,3?</t>
+  </si>
+  <si>
+    <t>planktic sheet-forming colonial algae</t>
   </si>
 </sst>
 </file>
@@ -1630,8 +1633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC34C16-BDAC-5F40-B6B3-028EA14891F7}">
   <dimension ref="A1:D124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="C98" sqref="C98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2212,7 +2215,7 @@
         <v>16</v>
       </c>
       <c r="B85" t="s">
-        <v>17</v>
+        <v>179</v>
       </c>
       <c r="C85">
         <v>1</v>
@@ -2264,32 +2267,32 @@
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A92">
+      <c r="C92" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D92" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93">
         <v>18</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B93" t="s">
         <v>111</v>
       </c>
-      <c r="C92">
+      <c r="C93">
         <v>5</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C93" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C94" s="1" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C95" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D95" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Some fixes to Rhynie guild and taxa list files, including interaction updates
</commit_message>
<xml_diff>
--- a/RhynieGuildStructure.xlsx
+++ b/RhynieGuildStructure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tannerfrank/Dropbox/Work/Devonian terr ecosystems/EcolNetworks/RhynieWebRepo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tannerfrank/Library/CloudStorage/Dropbox/Work/Devonian terr ecosystems/EcolNetworks/RhynieWebRepo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21498FD4-B9F6-594A-9051-BEC7B1935A4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E72B9FF4-8240-2345-B733-E1502904EBCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18800" yWindow="680" windowWidth="10000" windowHeight="16460" activeTab="1" xr2:uid="{917E407B-513B-1147-91E2-A7CD7550F694}"/>
+    <workbookView xWindow="18800" yWindow="680" windowWidth="17000" windowHeight="19360" xr2:uid="{917E407B-513B-1147-91E2-A7CD7550F694}"/>
   </bookViews>
   <sheets>
     <sheet name="Guilds" sheetId="3" r:id="rId1"/>
@@ -964,8 +964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63A68499-41B5-0044-B3AC-D073A84B94F6}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1074,7 +1074,7 @@
         <v>138</v>
       </c>
       <c r="D5" s="2">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E5" s="2">
         <v>1</v>
@@ -1451,7 +1451,7 @@
         <v>136</v>
       </c>
       <c r="D22" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E22" s="2">
         <v>13</v>
@@ -1633,8 +1633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC34C16-BDAC-5F40-B6B3-028EA14891F7}">
   <dimension ref="A1:D124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="C98" sqref="C98"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1759,17 +1759,17 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C17" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C18" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C19" s="1" t="s">
         <v>64</v>
       </c>
@@ -1777,7 +1777,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="3:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C20" s="1" t="s">
         <v>65</v>
       </c>
@@ -1785,7 +1785,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="3:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C21" s="1" t="s">
         <v>66</v>
       </c>
@@ -1793,7 +1793,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="3:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C22" s="1" t="s">
         <v>67</v>
       </c>
@@ -1801,7 +1801,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="3:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C23" s="1" t="s">
         <v>68</v>
       </c>
@@ -1809,7 +1809,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="3:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C24" s="1" t="s">
         <v>69</v>
       </c>
@@ -1817,429 +1817,432 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="3:4" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="C25" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C26" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C27" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C28" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C29" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C30" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C31" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="32" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C32" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D31" t="s">
         <v>42</v>
       </c>
     </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>5</v>
+      </c>
+      <c r="B32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32">
+        <v>9</v>
+      </c>
+    </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>5</v>
-      </c>
-      <c r="B33" t="s">
-        <v>2</v>
-      </c>
-      <c r="C33">
-        <v>9</v>
+      <c r="C33" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C34" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C35" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C36" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="C37" s="1" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
     </row>
     <row r="38" spans="1:4" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="C38" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="39" spans="1:4" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="C39" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="40" spans="1:4" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="C40" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="41" spans="1:4" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="C41" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="C42" s="1" t="s">
         <v>88</v>
       </c>
     </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>6</v>
+      </c>
+      <c r="B42" t="s">
+        <v>18</v>
+      </c>
+      <c r="C42">
+        <v>7</v>
+      </c>
+    </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <v>6</v>
-      </c>
-      <c r="B43" t="s">
-        <v>18</v>
-      </c>
-      <c r="C43">
-        <v>7</v>
+      <c r="C43" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D43" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C44" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D44" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="C45" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C45" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="46" spans="1:4" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="C46" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>42</v>
+        <v>78</v>
       </c>
     </row>
     <row r="47" spans="1:4" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="C47" s="1" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
     </row>
     <row r="48" spans="1:4" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="C48" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="49" spans="1:4" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="C49" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="C50" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="D49" s="1" t="s">
         <v>42</v>
       </c>
     </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>7</v>
+      </c>
+      <c r="B50" t="s">
+        <v>19</v>
+      </c>
+      <c r="C50">
+        <v>3</v>
+      </c>
+    </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51">
-        <v>7</v>
-      </c>
-      <c r="B51" t="s">
-        <v>19</v>
-      </c>
-      <c r="C51">
-        <v>3</v>
+      <c r="C51" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C52" s="1" t="s">
-        <v>75</v>
+        <v>81</v>
+      </c>
+      <c r="D52" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C53" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D53" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>8</v>
+      </c>
+      <c r="B54" t="s">
+        <v>4</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C55" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>9</v>
+      </c>
+      <c r="B56" t="s">
+        <v>3</v>
+      </c>
+      <c r="C56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C57" t="s">
+        <v>49</v>
+      </c>
+      <c r="D57" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C54" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55">
-        <v>8</v>
-      </c>
-      <c r="B55" t="s">
-        <v>4</v>
-      </c>
-      <c r="C55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C56" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57">
-        <v>9</v>
-      </c>
-      <c r="B57" t="s">
-        <v>3</v>
-      </c>
-      <c r="C57">
-        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C58" t="s">
-        <v>49</v>
-      </c>
-      <c r="D58" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>10</v>
+      </c>
+      <c r="B59" t="s">
+        <v>175</v>
+      </c>
+      <c r="C59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C60" t="s">
+        <v>56</v>
+      </c>
+      <c r="D60" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C59" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60">
-        <v>10</v>
-      </c>
-      <c r="B60" t="s">
-        <v>175</v>
-      </c>
-      <c r="C60">
-        <v>2</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C61" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D61" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C62" t="s">
-        <v>57</v>
-      </c>
-      <c r="D62" t="s">
-        <v>42</v>
+      <c r="A62">
+        <v>11</v>
+      </c>
+      <c r="B62" t="s">
+        <v>5</v>
+      </c>
+      <c r="C62">
+        <v>3</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63">
-        <v>11</v>
-      </c>
-      <c r="B63" t="s">
-        <v>5</v>
-      </c>
-      <c r="C63">
-        <v>3</v>
+      <c r="C63" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C64" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C65" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C66" t="s">
-        <v>54</v>
+      <c r="A66">
+        <v>12</v>
+      </c>
+      <c r="B66" t="s">
+        <v>6</v>
+      </c>
+      <c r="C66">
+        <v>5</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67">
-        <v>12</v>
-      </c>
-      <c r="B67" t="s">
-        <v>6</v>
-      </c>
-      <c r="C67">
-        <v>5</v>
+      <c r="C67" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C68" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C69" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C70" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C71" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C72" t="s">
-        <v>52</v>
+      <c r="A72">
+        <v>13</v>
+      </c>
+      <c r="B72" t="s">
+        <v>7</v>
+      </c>
+      <c r="C72">
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73">
-        <v>13</v>
-      </c>
-      <c r="B73" t="s">
-        <v>7</v>
-      </c>
-      <c r="C73">
-        <v>1</v>
+      <c r="C73" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C74" t="s">
-        <v>103</v>
+      <c r="A74">
+        <v>14</v>
+      </c>
+      <c r="B74" t="s">
+        <v>24</v>
+      </c>
+      <c r="C74">
+        <v>3</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75">
-        <v>14</v>
-      </c>
-      <c r="B75" t="s">
-        <v>24</v>
-      </c>
-      <c r="C75">
-        <v>3</v>
+      <c r="C75" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C76" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C77" t="s">
-        <v>121</v>
+      <c r="C77" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C78" s="1" t="s">
-        <v>13</v>
+      <c r="A78">
+        <v>15</v>
+      </c>
+      <c r="B78" t="s">
+        <v>113</v>
+      </c>
+      <c r="C78">
+        <v>5</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79">
-        <v>15</v>
-      </c>
-      <c r="B79" t="s">
-        <v>113</v>
-      </c>
-      <c r="C79">
-        <v>5</v>
+      <c r="C79" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D79" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C80" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D80" t="s">
-        <v>42</v>
+        <v>114</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C81" s="1" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C82" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C83" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C84" s="1" t="s">
-        <v>128</v>
+      <c r="A84">
+        <v>16</v>
+      </c>
+      <c r="B84" t="s">
+        <v>179</v>
+      </c>
+      <c r="C84">
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A85">
-        <v>16</v>
-      </c>
-      <c r="B85" t="s">
-        <v>179</v>
-      </c>
-      <c r="C85">
-        <v>1</v>
+      <c r="C85" s="1" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C86" s="1" t="s">
-        <v>131</v>
+      <c r="A86">
+        <v>17</v>
+      </c>
+      <c r="B86" t="s">
+        <v>8</v>
+      </c>
+      <c r="C86">
+        <v>4</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A87">
-        <v>17</v>
-      </c>
-      <c r="B87" t="s">
-        <v>8</v>
-      </c>
-      <c r="C87">
-        <v>4</v>
+      <c r="C87" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D87" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C88" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D88" t="s">
         <v>110</v>
@@ -2247,115 +2250,112 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C89" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D89" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C90" s="1" t="s">
-        <v>122</v>
+        <v>129</v>
+      </c>
+      <c r="D90" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C91" s="1" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="D91" t="s">
-        <v>42</v>
+        <v>117</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C92" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D92" t="s">
-        <v>117</v>
+      <c r="A92">
+        <v>18</v>
+      </c>
+      <c r="B92" t="s">
+        <v>111</v>
+      </c>
+      <c r="C92">
+        <v>5</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A93">
-        <v>18</v>
-      </c>
-      <c r="B93" t="s">
-        <v>111</v>
-      </c>
-      <c r="C93">
-        <v>5</v>
+      <c r="C93" s="1" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C94" s="1" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C95" s="1" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C96" s="1" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C97" s="1" t="s">
-        <v>132</v>
+      <c r="A97">
+        <v>19</v>
+      </c>
+      <c r="B97" t="s">
+        <v>9</v>
+      </c>
+      <c r="C97">
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A98">
-        <v>19</v>
-      </c>
-      <c r="B98" t="s">
-        <v>9</v>
-      </c>
-      <c r="C98">
-        <v>1</v>
+      <c r="C98" s="1" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C99" s="1" t="s">
-        <v>107</v>
+      <c r="A99">
+        <v>20</v>
+      </c>
+      <c r="B99" t="s">
+        <v>112</v>
+      </c>
+      <c r="C99" s="1">
+        <v>3</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A100">
-        <v>20</v>
-      </c>
-      <c r="B100" t="s">
-        <v>112</v>
-      </c>
-      <c r="C100" s="1">
-        <v>3</v>
+      <c r="C100" s="1" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C101" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C102" s="1" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C103" s="1" t="s">
-        <v>130</v>
+      <c r="A103">
+        <v>21</v>
+      </c>
+      <c r="B103" t="s">
+        <v>22</v>
+      </c>
+      <c r="C103">
+        <v>4</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A104">
-        <v>21</v>
-      </c>
-      <c r="B104" t="s">
-        <v>22</v>
-      </c>
-      <c r="C104">
-        <v>4</v>
+      <c r="C104" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
various updates including adding LittleRockLake date
</commit_message>
<xml_diff>
--- a/RhynieGuildStructure.xlsx
+++ b/RhynieGuildStructure.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tannerfrank/Library/CloudStorage/Dropbox/Work/Devonian terr ecosystems/EcolNetworks/RhynieWebRepo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E72B9FF4-8240-2345-B733-E1502904EBCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B70A3C44-44EA-F448-8033-D0C568FD5396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18800" yWindow="680" windowWidth="17000" windowHeight="19360" xr2:uid="{917E407B-513B-1147-91E2-A7CD7550F694}"/>
   </bookViews>
@@ -965,7 +965,7 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1120,7 +1120,7 @@
         <v>136</v>
       </c>
       <c r="D7" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>79</v>
@@ -1143,7 +1143,7 @@
         <v>136</v>
       </c>
       <c r="D8" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>177</v>
@@ -1633,8 +1633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC34C16-BDAC-5F40-B6B3-028EA14891F7}">
   <dimension ref="A1:D124"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1919,7 +1919,7 @@
         <v>18</v>
       </c>
       <c r="C42">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -1937,44 +1937,44 @@
     </row>
     <row r="45" spans="1:4" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="C45" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>42</v>
+        <v>78</v>
       </c>
     </row>
     <row r="46" spans="1:4" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="C46" s="1" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
     </row>
     <row r="47" spans="1:4" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="C47" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="48" spans="1:4" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="C48" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="C49" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="D48" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49">
         <v>7</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B49" t="s">
         <v>19</v>
       </c>
-      <c r="C50">
-        <v>3</v>
+      <c r="C49">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="C50" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>